<commit_message>
new database + borrower
</commit_message>
<xml_diff>
--- a/library_Database.xlsx
+++ b/library_Database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>Borrower</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>copyNo(int)</t>
+  </si>
+  <si>
+    <t>Fine</t>
   </si>
 </sst>
 </file>
@@ -643,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -955,6 +958,13 @@
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
@@ -1223,13 +1233,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="H7:K7"/>
+    <mergeCell ref="E13:I13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished implementing add borrower function
</commit_message>
<xml_diff>
--- a/library_Database.xlsx
+++ b/library_Database.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="19440" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="22760" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Borrower</t>
   </si>
@@ -252,13 +257,36 @@
   </si>
   <si>
     <t>Fine</t>
+  </si>
+  <si>
+    <t>password4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Barack Obama</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Washington DC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>obama@gmail.com</t>
+  </si>
+  <si>
+    <t>69-12-12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +318,13 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -308,10 +343,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -331,6 +370,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,12 +385,16 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -643,45 +689,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:I13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="K1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="12"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
@@ -817,21 +863,50 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="9">
+        <v>98765432</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="9">
+        <v>999999</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="H7" s="11" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="H7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
@@ -953,18 +1028,18 @@
       <c r="G11" s="1"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="E13" s="11" t="s">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="E13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
@@ -1126,14 +1201,14 @@
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
@@ -1243,33 +1318,50 @@
     <mergeCell ref="E13:I13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated excel and tested Clerk
</commit_message>
<xml_diff>
--- a/library_Database.xlsx
+++ b/library_Database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="22760" windowHeight="8020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24220" windowHeight="10120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
   <si>
     <t>Borrower</t>
   </si>
@@ -164,9 +164,6 @@
     <t>out</t>
   </si>
   <si>
-    <t>on-hold</t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
@@ -279,6 +276,14 @@
   </si>
   <si>
     <t>Stu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>on hold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>on hold</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -350,7 +355,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,6 +378,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -385,8 +396,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -690,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -713,21 +724,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="K1" s="13" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="K1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="13"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
@@ -868,45 +879,45 @@
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="E6" s="9">
         <v>98765432</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>77</v>
+      <c r="F6" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="G6" s="9">
         <v>999999</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="H7" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="H7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
@@ -928,7 +939,7 @@
         <v>44</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>4</v>
@@ -937,7 +948,7 @@
         <v>26</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -961,7 +972,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I9">
         <v>11111111</v>
@@ -970,7 +981,7 @@
         <v>1001</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -994,7 +1005,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10">
         <v>22222222</v>
@@ -1003,7 +1014,7 @@
         <v>2002</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1028,43 +1039,43 @@
       <c r="G11" s="1"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="E13" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" t="s">
         <v>66</v>
-      </c>
-      <c r="I14" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1074,8 +1085,8 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>46</v>
+      <c r="C15" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1087,7 +1098,7 @@
         <v>41255</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1100,8 +1111,8 @@
       <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
+      <c r="C16" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1113,7 +1124,7 @@
         <v>41275</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -1139,7 +1150,7 @@
         <v>41275</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -1153,7 +1164,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1164,7 +1175,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1175,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1186,7 +1197,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1197,48 +1208,48 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="A24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
         <v>56</v>
       </c>
-      <c r="D25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26">
         <v>11111111</v>
       </c>
       <c r="C26">
-        <v>1001</v>
+        <v>2002</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1250,61 +1261,84 @@
         <v>41365</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="14" customHeight="1">
       <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27">
-        <v>11111111</v>
+        <v>1</v>
+      </c>
+      <c r="B27" s="16">
+        <v>5555555</v>
       </c>
       <c r="C27">
-        <v>2002</v>
+        <v>1001</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27" s="7">
-        <v>41359</v>
+        <v>41364</v>
       </c>
       <c r="F27" s="7">
-        <v>41365</v>
+        <v>41378</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>22222222</v>
+        <v>5555555</v>
       </c>
       <c r="C28">
         <v>1001</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E28" s="7">
-        <v>41359</v>
+        <v>41364</v>
       </c>
       <c r="F28" s="7">
-        <v>41360</v>
+        <v>41347</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B29">
-        <v>22222222</v>
+        <v>5555555</v>
       </c>
       <c r="C29">
-        <v>1001</v>
+        <v>3003</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E29" s="7">
-        <v>41359</v>
+        <v>41364</v>
+      </c>
+      <c r="F29" s="7">
+        <v>41347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>5555555</v>
+      </c>
+      <c r="C30">
+        <v>2002</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7">
+        <v>41364</v>
+      </c>
+      <c r="F30" s="7">
+        <v>41347</v>
       </c>
     </row>
   </sheetData>
@@ -1322,6 +1356,7 @@
     <hyperlink ref="F6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
made it to match our datatbase
</commit_message>
<xml_diff>
--- a/library_Database.xlsx
+++ b/library_Database.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24480" windowHeight="15320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
   <si>
     <t>Borrower</t>
   </si>
@@ -268,10 +268,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Stu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>on hold</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -296,7 +292,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>in</t>
+    <t>Student</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -308,7 +304,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -316,13 +312,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -331,7 +327,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -368,7 +364,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,6 +393,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -410,7 +409,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -713,45 +715,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="K1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="K1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
@@ -894,7 +896,7 @@
       <c r="B6" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -913,24 +915,24 @@
         <v>75</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="H7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
@@ -1051,7 +1053,7 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11">
         <v>11111111</v>
@@ -1060,22 +1062,22 @@
         <v>3003</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="E13" s="14" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="E13" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
@@ -1111,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1137,7 +1139,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1162,8 +1164,8 @@
       <c r="B17" s="1">
         <v>3</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>83</v>
+      <c r="C17" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="E17">
         <v>6</v>
@@ -1222,7 +1224,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1233,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1244,18 +1246,18 @@
         <v>1</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
@@ -1278,103 +1280,123 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26">
+      <c r="A26" s="17">
+        <v>4</v>
+      </c>
+      <c r="B26" s="17">
+        <v>5555555</v>
+      </c>
+      <c r="C26" s="17">
+        <v>1001</v>
+      </c>
+      <c r="D26" s="17">
+        <v>5</v>
+      </c>
+      <c r="E26" s="18">
+        <v>41364</v>
+      </c>
+      <c r="F26" s="18">
+        <v>41377</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.1" customHeight="1">
+      <c r="A27" s="17">
+        <v>5</v>
+      </c>
+      <c r="B27" s="17">
+        <v>5555555</v>
+      </c>
+      <c r="C27" s="17">
+        <v>3003</v>
+      </c>
+      <c r="D27" s="17">
+        <v>1</v>
+      </c>
+      <c r="E27" s="18">
+        <v>41364</v>
+      </c>
+      <c r="F27" s="18">
+        <v>41377</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="17">
+        <v>6</v>
+      </c>
+      <c r="B28" s="17">
+        <v>5555555</v>
+      </c>
+      <c r="C28" s="17">
+        <v>2002</v>
+      </c>
+      <c r="D28" s="17">
         <v>2</v>
       </c>
-      <c r="B26">
+      <c r="E28" s="18">
+        <v>41364</v>
+      </c>
+      <c r="F28" s="18">
+        <v>41377</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="17">
+        <v>2</v>
+      </c>
+      <c r="B29" s="17">
         <v>11111111</v>
       </c>
-      <c r="C26">
+      <c r="C29" s="17">
         <v>2002</v>
       </c>
-      <c r="D26">
+      <c r="D29" s="17">
         <v>1</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E29" s="18">
         <v>41359</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F29" s="18">
         <v>41365</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14" customHeight="1">
-      <c r="A27">
+    <row r="30" spans="1:9">
+      <c r="A30" s="17">
+        <v>3</v>
+      </c>
+      <c r="B30" s="17">
+        <v>22222222</v>
+      </c>
+      <c r="C30" s="17">
+        <v>1001</v>
+      </c>
+      <c r="D30" s="17">
+        <v>2</v>
+      </c>
+      <c r="E30" s="18">
+        <v>41359</v>
+      </c>
+      <c r="F30" s="18">
+        <v>41360</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="17">
         <v>1</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B31" s="17">
         <v>5555555</v>
       </c>
-      <c r="C27">
+      <c r="C31" s="17">
         <v>1001</v>
       </c>
-      <c r="D27">
+      <c r="D31" s="17">
         <v>4</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E31" s="18">
         <v>41364</v>
       </c>
-      <c r="F27" s="7">
-        <v>41378</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>5555555</v>
-      </c>
-      <c r="C28">
-        <v>1001</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28" s="7">
-        <v>41364</v>
-      </c>
-      <c r="F28" s="7">
-        <v>41347</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29">
-        <v>5</v>
-      </c>
-      <c r="B29">
-        <v>5555555</v>
-      </c>
-      <c r="C29">
-        <v>3003</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="7">
-        <v>41364</v>
-      </c>
-      <c r="F29" s="7">
-        <v>41347</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30">
-        <v>6</v>
-      </c>
-      <c r="B30">
-        <v>5555555</v>
-      </c>
-      <c r="C30">
-        <v>2002</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30" s="7">
-        <v>41364</v>
-      </c>
-      <c r="F30" s="7">
-        <v>41347</v>
+      <c r="F31" s="18">
+        <v>41377</v>
       </c>
     </row>
   </sheetData>
@@ -1402,12 +1424,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1420,12 +1442,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>